<commit_message>
Create logic to build dashboard
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/Bowl Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183F717E-B9B7-FA4D-BA24-65AC29FE6AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0A285-54B8-CF46-AEB6-7A73B90AF063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="250">
   <si>
     <t>School</t>
   </si>
@@ -516,9 +519,6 @@
     <t>Central Michigan</t>
   </si>
   <si>
-    <t>FAU</t>
-  </si>
-  <si>
     <t>SMU</t>
   </si>
   <si>
@@ -534,9 +534,6 @@
     <t>Boise State</t>
   </si>
   <si>
-    <t>App State</t>
-  </si>
-  <si>
     <t>Eastern Michigan</t>
   </si>
   <si>
@@ -573,9 +570,6 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>Cal</t>
-  </si>
-  <si>
     <t>Louisville</t>
   </si>
   <si>
@@ -666,9 +660,6 @@
     <t>Fighting Illini</t>
   </si>
   <si>
-    <t>Bruins</t>
-  </si>
-  <si>
     <t>Cavaliers</t>
   </si>
   <si>
@@ -784,6 +775,12 @@
   </si>
   <si>
     <t>Georgia Tech</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Golden Bears</t>
   </si>
 </sst>
 </file>
@@ -1626,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="N215" sqref="N136:N215"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3895,7 +3892,7 @@
         <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C56">
         <v>2019</v>
@@ -3977,7 +3974,7 @@
         <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C58">
         <v>2019</v>
@@ -4059,7 +4056,7 @@
         <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C60">
         <v>2019</v>
@@ -4100,7 +4097,7 @@
         <v>161</v>
       </c>
       <c r="B61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C61">
         <v>2019</v>
@@ -4220,7 +4217,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
         <v>61</v>
@@ -4232,7 +4229,7 @@
         <v>39</v>
       </c>
       <c r="E64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F64">
         <v>52</v>
@@ -4261,10 +4258,10 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C65">
         <v>2019</v>
@@ -4273,7 +4270,7 @@
         <v>39</v>
       </c>
       <c r="E65" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
       <c r="F65">
         <v>28</v>
@@ -4302,10 +4299,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B66" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C66">
         <v>2019</v>
@@ -4314,7 +4311,7 @@
         <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F66">
         <v>34</v>
@@ -4343,7 +4340,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -4355,7 +4352,7 @@
         <v>35</v>
       </c>
       <c r="E67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F67">
         <v>26</v>
@@ -4384,10 +4381,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C68">
         <v>2019</v>
@@ -4396,7 +4393,7 @@
         <v>139</v>
       </c>
       <c r="E68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F68">
         <v>38</v>
@@ -4425,10 +4422,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C69">
         <v>2019</v>
@@ -4437,7 +4434,7 @@
         <v>139</v>
       </c>
       <c r="E69" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F69">
         <v>7</v>
@@ -4478,7 +4475,7 @@
         <v>67</v>
       </c>
       <c r="E70" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="F70">
         <v>17</v>
@@ -4507,7 +4504,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
         <v>18</v>
@@ -4794,7 +4791,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
         <v>66</v>
@@ -4806,7 +4803,7 @@
         <v>142</v>
       </c>
       <c r="E78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F78">
         <v>30</v>
@@ -4835,7 +4832,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
         <v>70</v>
@@ -4847,7 +4844,7 @@
         <v>142</v>
       </c>
       <c r="E79" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F79">
         <v>34</v>
@@ -4876,7 +4873,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
         <v>38</v>
@@ -4888,7 +4885,7 @@
         <v>97</v>
       </c>
       <c r="E80" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F80">
         <v>21</v>
@@ -4917,10 +4914,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C81">
         <v>2019</v>
@@ -4929,7 +4926,7 @@
         <v>97</v>
       </c>
       <c r="E81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F81">
         <v>31</v>
@@ -4958,7 +4955,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B82" t="s">
         <v>61</v>
@@ -5011,7 +5008,7 @@
         <v>143</v>
       </c>
       <c r="E83" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F83">
         <v>55</v>
@@ -5052,7 +5049,7 @@
         <v>144</v>
       </c>
       <c r="E84" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F84">
         <v>21</v>
@@ -5081,10 +5078,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B85" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C85">
         <v>2019</v>
@@ -5204,10 +5201,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C88">
         <v>2019</v>
@@ -5216,7 +5213,7 @@
         <v>146</v>
       </c>
       <c r="E88" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F88">
         <v>49</v>
@@ -5245,10 +5242,10 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B89" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C89">
         <v>2019</v>
@@ -5257,7 +5254,7 @@
         <v>146</v>
       </c>
       <c r="E89" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F89">
         <v>24</v>
@@ -5368,10 +5365,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B92" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C92">
         <v>2019</v>
@@ -5421,7 +5418,7 @@
         <v>148</v>
       </c>
       <c r="E93" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F93">
         <v>39</v>
@@ -5450,7 +5447,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B94" t="s">
         <v>26</v>
@@ -5503,7 +5500,7 @@
         <v>43</v>
       </c>
       <c r="E95" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F95">
         <v>28</v>
@@ -5614,10 +5611,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C98">
         <v>2019</v>
@@ -5667,7 +5664,7 @@
         <v>149</v>
       </c>
       <c r="E99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F99">
         <v>23</v>
@@ -5696,10 +5693,10 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B100" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C100">
         <v>2019</v>
@@ -5708,7 +5705,7 @@
         <v>150</v>
       </c>
       <c r="E100" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="F100">
         <v>20</v>
@@ -5737,10 +5734,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="B101" t="s">
-        <v>212</v>
+        <v>249</v>
       </c>
       <c r="C101">
         <v>2019</v>
@@ -5749,7 +5746,7 @@
         <v>150</v>
       </c>
       <c r="E101" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F101">
         <v>35</v>
@@ -5778,7 +5775,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B102" t="s">
         <v>30</v>
@@ -5831,7 +5828,7 @@
         <v>151</v>
       </c>
       <c r="E103" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F103">
         <v>28</v>
@@ -5860,10 +5857,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B104" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C104">
         <v>2019</v>
@@ -5913,7 +5910,7 @@
         <v>110</v>
       </c>
       <c r="E105" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F105">
         <v>36</v>
@@ -5954,7 +5951,7 @@
         <v>152</v>
       </c>
       <c r="E106" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F106">
         <v>22</v>
@@ -5983,10 +5980,10 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C107">
         <v>2019</v>
@@ -6024,10 +6021,10 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C108">
         <v>2019</v>
@@ -6036,7 +6033,7 @@
         <v>153</v>
       </c>
       <c r="E108" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F108">
         <v>20</v>
@@ -6065,10 +6062,10 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C109">
         <v>2019</v>
@@ -6077,7 +6074,7 @@
         <v>153</v>
       </c>
       <c r="E109" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F109">
         <v>14</v>
@@ -6106,7 +6103,7 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B110" t="s">
         <v>86</v>
@@ -6118,7 +6115,7 @@
         <v>23</v>
       </c>
       <c r="E110" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F110">
         <v>17</v>
@@ -6147,10 +6144,10 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B111" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C111">
         <v>2019</v>
@@ -6159,7 +6156,7 @@
         <v>23</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F111">
         <v>20</v>
@@ -6200,7 +6197,7 @@
         <v>31</v>
       </c>
       <c r="E112" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F112">
         <v>17</v>
@@ -6229,7 +6226,7 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B113" t="s">
         <v>116</v>
@@ -6282,7 +6279,7 @@
         <v>54</v>
       </c>
       <c r="E114" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F114">
         <v>38</v>
@@ -6311,10 +6308,10 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B115" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C115">
         <v>2019</v>
@@ -6364,7 +6361,7 @@
         <v>27</v>
       </c>
       <c r="E116" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F116">
         <v>35</v>
@@ -6393,10 +6390,10 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B117" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C117">
         <v>2019</v>
@@ -6446,7 +6443,7 @@
         <v>79</v>
       </c>
       <c r="E118" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F118">
         <v>24</v>
@@ -6475,10 +6472,10 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B119" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C119">
         <v>2019</v>
@@ -6598,10 +6595,10 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B122" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C122">
         <v>2019</v>
@@ -6651,7 +6648,7 @@
         <v>46</v>
       </c>
       <c r="E123" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F123">
         <v>26</v>
@@ -6692,7 +6689,7 @@
         <v>154</v>
       </c>
       <c r="E124" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F124">
         <v>38</v>
@@ -6721,7 +6718,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B125" t="s">
         <v>66</v>
@@ -6762,10 +6759,10 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B126" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C126">
         <v>2019</v>
@@ -6815,7 +6812,7 @@
         <v>87</v>
       </c>
       <c r="E127" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F127">
         <v>22</v>
@@ -6856,7 +6853,7 @@
         <v>155</v>
       </c>
       <c r="E128" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F128">
         <v>21</v>
@@ -6885,10 +6882,10 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B129" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C129">
         <v>2019</v>
@@ -6938,7 +6935,7 @@
         <v>101</v>
       </c>
       <c r="E130" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F130">
         <v>30</v>
@@ -6967,10 +6964,10 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B131" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C131">
         <v>2019</v>
@@ -7008,10 +7005,10 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B132" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C132">
         <v>2019</v>
@@ -7061,7 +7058,7 @@
         <v>156</v>
       </c>
       <c r="E133" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F133">
         <v>27</v>
@@ -7090,7 +7087,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
         <v>26</v>
@@ -7143,7 +7140,7 @@
         <v>136</v>
       </c>
       <c r="E135" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F135">
         <v>25</v>
@@ -7264,10 +7261,10 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C140">
         <v>2018</v>
@@ -7276,7 +7273,7 @@
         <v>139</v>
       </c>
       <c r="E140" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F140">
         <v>20</v>
@@ -7287,7 +7284,7 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B141" t="s">
         <v>64</v>
@@ -7299,7 +7296,7 @@
         <v>139</v>
       </c>
       <c r="E141" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F141">
         <v>31</v>
@@ -7310,7 +7307,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B142" t="s">
         <v>66</v>
@@ -7345,7 +7342,7 @@
         <v>35</v>
       </c>
       <c r="E143" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F143">
         <v>23</v>
@@ -7356,7 +7353,7 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="B144" t="s">
         <v>18</v>
@@ -7368,7 +7365,7 @@
         <v>67</v>
       </c>
       <c r="E144" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F144">
         <v>45</v>
@@ -7379,10 +7376,10 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B145" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C145">
         <v>2018</v>
@@ -7391,7 +7388,7 @@
         <v>67</v>
       </c>
       <c r="E145" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="F145">
         <v>13</v>
@@ -7414,7 +7411,7 @@
         <v>39</v>
       </c>
       <c r="E146" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F146">
         <v>37</v>
@@ -7425,10 +7422,10 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B147" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C147">
         <v>2018</v>
@@ -7448,10 +7445,10 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B148" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C148">
         <v>2018</v>
@@ -7474,7 +7471,7 @@
         <v>160</v>
       </c>
       <c r="B149" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C149">
         <v>2018</v>
@@ -7483,7 +7480,7 @@
         <v>138</v>
       </c>
       <c r="E149" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F149">
         <v>0</v>
@@ -7506,7 +7503,7 @@
         <v>121</v>
       </c>
       <c r="E150" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F150">
         <v>38</v>
@@ -7517,7 +7514,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B151" t="s">
         <v>34</v>
@@ -7540,10 +7537,10 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B152" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C152">
         <v>2018</v>
@@ -7552,7 +7549,7 @@
         <v>137</v>
       </c>
       <c r="E152" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F152">
         <v>32</v>
@@ -7563,7 +7560,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B153" t="s">
         <v>70</v>
@@ -7575,7 +7572,7 @@
         <v>137</v>
       </c>
       <c r="E153" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F153">
         <v>35</v>
@@ -7598,7 +7595,7 @@
         <v>155</v>
       </c>
       <c r="E154" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F154">
         <v>49</v>
@@ -7609,10 +7606,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B155" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C155">
         <v>2018</v>
@@ -7733,10 +7730,10 @@
         <v>2018</v>
       </c>
       <c r="D160" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E160" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F160">
         <v>32</v>
@@ -7747,16 +7744,16 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B161" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C161">
         <v>2018</v>
       </c>
       <c r="D161" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E161" t="s">
         <v>33</v>
@@ -7816,7 +7813,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B164" t="s">
         <v>66</v>
@@ -7828,7 +7825,7 @@
         <v>92</v>
       </c>
       <c r="E164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F164">
         <v>0</v>
@@ -7839,10 +7836,10 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B165" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C165">
         <v>2018</v>
@@ -7851,7 +7848,7 @@
         <v>92</v>
       </c>
       <c r="E165" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F165">
         <v>0</v>
@@ -7862,10 +7859,10 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B166" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C166">
         <v>2018</v>
@@ -7885,10 +7882,10 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B167" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C167">
         <v>2018</v>
@@ -7897,7 +7894,7 @@
         <v>142</v>
       </c>
       <c r="E167" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F167">
         <v>10</v>
@@ -7908,19 +7905,19 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B168" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C168">
         <v>2018</v>
       </c>
       <c r="D168" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E168" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="F168">
         <v>10</v>
@@ -7931,19 +7928,19 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="B169" t="s">
-        <v>212</v>
+        <v>249</v>
       </c>
       <c r="C169">
         <v>2018</v>
       </c>
       <c r="D169" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E169" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F169">
         <v>7</v>
@@ -7954,7 +7951,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B170" t="s">
         <v>61</v>
@@ -7966,7 +7963,7 @@
         <v>141</v>
       </c>
       <c r="E170" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F170">
         <v>27</v>
@@ -7977,10 +7974,10 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B171" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C171">
         <v>2018</v>
@@ -7989,7 +7986,7 @@
         <v>141</v>
       </c>
       <c r="E171" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F171">
         <v>56</v>
@@ -8046,10 +8043,10 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B174" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C174">
         <v>2018</v>
@@ -8058,7 +8055,7 @@
         <v>145</v>
       </c>
       <c r="E174" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F174">
         <v>45</v>
@@ -8069,10 +8066,10 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B175" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C175">
         <v>2018</v>
@@ -8081,7 +8078,7 @@
         <v>145</v>
       </c>
       <c r="E175" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F175">
         <v>38</v>
@@ -8104,7 +8101,7 @@
         <v>151</v>
       </c>
       <c r="E176" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F176">
         <v>63</v>
@@ -8115,10 +8112,10 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B177" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C177">
         <v>2018</v>
@@ -8150,7 +8147,7 @@
         <v>147</v>
       </c>
       <c r="E178" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F178">
         <v>18</v>
@@ -8161,10 +8158,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B179" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C179">
         <v>2018</v>
@@ -8196,7 +8193,7 @@
         <v>54</v>
       </c>
       <c r="E180" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F180">
         <v>26</v>
@@ -8207,7 +8204,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B181" t="s">
         <v>38</v>
@@ -8322,10 +8319,10 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C186">
         <v>2018</v>
@@ -8357,7 +8354,7 @@
         <v>43</v>
       </c>
       <c r="E187" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F187">
         <v>41</v>
@@ -8380,7 +8377,7 @@
         <v>152</v>
       </c>
       <c r="E188" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F188">
         <v>0</v>
@@ -8391,10 +8388,10 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B189" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C189">
         <v>2018</v>
@@ -8426,7 +8423,7 @@
         <v>31</v>
       </c>
       <c r="E190" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F190">
         <v>16</v>
@@ -8437,10 +8434,10 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B191" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C191">
         <v>2018</v>
@@ -8472,7 +8469,7 @@
         <v>143</v>
       </c>
       <c r="E192" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F192">
         <v>35</v>
@@ -8483,10 +8480,10 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B193" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C193">
         <v>2018</v>
@@ -8506,10 +8503,10 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B194" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C194">
         <v>2018</v>
@@ -8541,7 +8538,7 @@
         <v>150</v>
       </c>
       <c r="E195" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F195">
         <v>7</v>
@@ -8552,7 +8549,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B196" t="s">
         <v>26</v>
@@ -8587,7 +8584,7 @@
         <v>23</v>
       </c>
       <c r="E197" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F197">
         <v>38</v>
@@ -8610,7 +8607,7 @@
         <v>146</v>
       </c>
       <c r="E198" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F198">
         <v>31</v>
@@ -8621,10 +8618,10 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B199" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C199">
         <v>2018</v>
@@ -8653,7 +8650,7 @@
         <v>2018</v>
       </c>
       <c r="D200" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E200" t="s">
         <v>88</v>
@@ -8676,7 +8673,7 @@
         <v>2018</v>
       </c>
       <c r="D201" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E201" t="s">
         <v>111</v>
@@ -8690,7 +8687,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B202" t="s">
         <v>70</v>
@@ -8702,7 +8699,7 @@
         <v>153</v>
       </c>
       <c r="E202" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F202">
         <v>13</v>
@@ -8713,10 +8710,10 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B203" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C203">
         <v>2018</v>
@@ -8725,7 +8722,7 @@
         <v>153</v>
       </c>
       <c r="E203" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F203">
         <v>14</v>
@@ -8782,7 +8779,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B206" t="s">
         <v>26</v>
@@ -8817,7 +8814,7 @@
         <v>83</v>
       </c>
       <c r="E207" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F207">
         <v>32</v>
@@ -8840,7 +8837,7 @@
         <v>15</v>
       </c>
       <c r="E208" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F208">
         <v>28</v>
@@ -8851,10 +8848,10 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B209" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C209">
         <v>2018</v>
@@ -8886,7 +8883,7 @@
         <v>79</v>
       </c>
       <c r="E210" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F210">
         <v>22</v>
@@ -8897,10 +8894,10 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B211" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C211">
         <v>2018</v>
@@ -8932,7 +8929,7 @@
         <v>27</v>
       </c>
       <c r="E212" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F212">
         <v>27</v>
@@ -8943,10 +8940,10 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B213" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C213">
         <v>2018</v>

</xml_diff>